<commit_message>
apply service offering acronyms/abbreviations to t1so, t2so
</commit_message>
<xml_diff>
--- a/testdata/K.xlsx
+++ b/testdata/K.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jisqhx3/automation/rulesBotGithubSyncVersion/omRules/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E83F71-1FEF-654E-8A86-F277DB203AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7290986-D783-9D4E-8201-2658706586C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="460" windowWidth="32680" windowHeight="20540" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Gold" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19539" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19550" uniqueCount="464">
   <si>
     <t>PARENT(Bill To, Fleet, Service Offering)</t>
   </si>
@@ -1398,9 +1398,6 @@
     <t>99BA11</t>
   </si>
   <si>
-    <t>Dedicated</t>
-  </si>
-  <si>
     <t>99KA9</t>
   </si>
   <si>
@@ -1432,6 +1429,18 @@
   </si>
   <si>
     <t>ALPI37</t>
+  </si>
+  <si>
+    <t>Dedi</t>
+  </si>
+  <si>
+    <t>OTR</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>Brok</t>
   </si>
 </sst>
 </file>
@@ -1649,11 +1658,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1661,17 +1670,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1685,10 +1685,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2020,22 +2029,22 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39" t="s">
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="39"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="5" t="s">
         <v>22</v>
       </c>
@@ -2084,19 +2093,19 @@
       <c r="Q3" s="9"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="36" t="s">
         <v>34</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -2110,17 +2119,17 @@
       <c r="M4" s="38"/>
       <c r="N4" s="32"/>
       <c r="O4" s="23"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="36" t="s">
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="46"/>
-      <c r="F5" s="42"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="10" t="s">
         <v>27</v>
       </c>
@@ -2132,8 +2141,8 @@
       <c r="M5" s="21"/>
       <c r="N5" s="32"/>
       <c r="O5" s="23"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="36"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="48"/>
     </row>
     <row r="6" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
@@ -2157,8 +2166,8 @@
       <c r="M6" s="8"/>
       <c r="N6" s="7"/>
       <c r="O6" s="8"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="36"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="48"/>
     </row>
     <row r="7" spans="1:17" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
@@ -2174,7 +2183,7 @@
         <v>35</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="36" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -2188,8 +2197,8 @@
       <c r="M7" s="38"/>
       <c r="N7" s="22"/>
       <c r="O7" s="23"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="36"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="48"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="29"/>
@@ -2197,7 +2206,7 @@
       <c r="C8" s="18"/>
       <c r="D8" s="19"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="42"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="10" t="s">
         <v>27</v>
       </c>
@@ -2209,8 +2218,8 @@
       <c r="M8" s="21"/>
       <c r="N8" s="22"/>
       <c r="O8" s="23"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="36"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="48"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
@@ -2222,8 +2231,8 @@
       <c r="K9" s="9"/>
       <c r="M9" s="9"/>
       <c r="O9" s="9"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="36"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="48"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
@@ -2231,7 +2240,7 @@
       <c r="C10" s="25"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="36" t="s">
         <v>39</v>
       </c>
       <c r="G10" s="10" t="s">
@@ -2245,8 +2254,8 @@
       <c r="M10" s="38"/>
       <c r="N10" s="22"/>
       <c r="O10" s="23"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="36"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="48"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
@@ -2254,7 +2263,7 @@
       <c r="C11" s="25"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="F11" s="42"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="10" t="s">
         <v>27</v>
       </c>
@@ -2266,8 +2275,8 @@
       <c r="M11" s="21"/>
       <c r="N11" s="22"/>
       <c r="O11" s="23"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="36"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="48"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C12" s="25"/>
@@ -2276,11 +2285,11 @@
       <c r="K12" s="9"/>
       <c r="M12" s="9"/>
       <c r="O12" s="9"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="36"/>
+      <c r="P12" s="47"/>
+      <c r="Q12" s="48"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="36" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="10" t="s">
@@ -2294,8 +2303,8 @@
       <c r="M13" s="38"/>
       <c r="N13" s="22"/>
       <c r="O13" s="23"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="36"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="48"/>
     </row>
     <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -2310,7 +2319,7 @@
       <c r="D14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="42"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="10" t="s">
         <v>27</v>
       </c>
@@ -2322,8 +2331,8 @@
       <c r="M14" s="21"/>
       <c r="N14" s="22"/>
       <c r="O14" s="23"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="36"/>
+      <c r="P14" s="47"/>
+      <c r="Q14" s="48"/>
     </row>
     <row r="15" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
@@ -2343,8 +2352,8 @@
       <c r="K15" s="9"/>
       <c r="M15" s="9"/>
       <c r="O15" s="9"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="36"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="48"/>
     </row>
     <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
@@ -2360,7 +2369,7 @@
         <v>37</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="36" t="s">
         <v>42</v>
       </c>
       <c r="G16" s="10" t="s">
@@ -2374,8 +2383,8 @@
       <c r="M16" s="38"/>
       <c r="N16" s="22"/>
       <c r="O16" s="23"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="36"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="48"/>
     </row>
     <row r="17" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
@@ -2391,7 +2400,7 @@
         <v>39</v>
       </c>
       <c r="E17" s="4"/>
-      <c r="F17" s="42"/>
+      <c r="F17" s="36"/>
       <c r="G17" s="10" t="s">
         <v>27</v>
       </c>
@@ -2403,8 +2412,8 @@
       <c r="M17" s="21"/>
       <c r="N17" s="22"/>
       <c r="O17" s="23"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="36"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="48"/>
     </row>
     <row r="18" spans="1:17" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
@@ -2443,22 +2452,22 @@
       <c r="G20" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="35" t="s">
         <v>421</v>
       </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="47"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="4"/>
       <c r="G21" t="s">
         <v>29</v>
       </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
@@ -2478,34 +2487,34 @@
     <sortCondition ref="C15:C19"/>
   </sortState>
   <mergeCells count="28">
+    <mergeCell ref="P4:P17"/>
+    <mergeCell ref="Q4:Q17"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="F16:F17"/>
     <mergeCell ref="J16:K16"/>
     <mergeCell ref="L16:M16"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="L13:M13"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="P4:P17"/>
-    <mergeCell ref="Q4:Q17"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2541,15 +2550,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -2557,10 +2566,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -2646,7 +2655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA3B3F7-C95A-8A4B-AD3C-BA266A349F38}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2668,10 +2677,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D2" t="s">
         <v>42</v>
@@ -78158,7 +78167,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C5"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -78237,7 +78246,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -78264,7 +78273,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>449</v>
+        <v>460</v>
       </c>
       <c r="B2" t="s">
         <v>443</v>
@@ -78272,7 +78281,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>449</v>
+        <v>460</v>
       </c>
       <c r="B3" t="s">
         <v>444</v>
@@ -78280,66 +78289,66 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>460</v>
+      </c>
+      <c r="B4" t="s">
         <v>449</v>
-      </c>
-      <c r="B4" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>449</v>
+        <v>460</v>
       </c>
       <c r="B5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="B6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="B7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="B8" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>449</v>
+        <v>461</v>
       </c>
       <c r="B9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="B10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>449</v>
+        <v>462</v>
       </c>
       <c r="B11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -78349,10 +78358,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9A0DBF-D3B6-4958-A13F-97CF8D4A51F7}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -78379,7 +78388,46 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>442</v>
+      </c>
+      <c r="B2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B3" t="s">
+        <v>444</v>
+      </c>
+      <c r="C3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C4" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>463</v>
+      </c>
+      <c r="B5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C5" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>

</xml_diff>